<commit_message>
Implemented the label and table tag
</commit_message>
<xml_diff>
--- a/src/main/resources/Template/Template.xlsx
+++ b/src/main/resources/Template/Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanojs\eclipse-workspace-panippura\WebAutomationAI\src\main\resources\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanojs\eclipse-workspace-snj\snj-web-inspect\src\main\resources\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16035" windowHeight="7470"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16035" windowHeight="7470" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="InputLocators" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,15 @@
     <sheet name="TextareaLocators" sheetId="3" r:id="rId3"/>
     <sheet name="DropDownLocators" sheetId="4" r:id="rId4"/>
     <sheet name="LinkLocators" sheetId="6" r:id="rId5"/>
+    <sheet name="LabelLocators" sheetId="7" r:id="rId6"/>
+    <sheet name="TableLocators" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="93">
   <si>
     <t>S.No</t>
   </si>
@@ -705,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1701,7 +1703,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2011,4 +2013,80 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the Web Inspect
</commit_message>
<xml_diff>
--- a/src/main/resources/Template/Template.xlsx
+++ b/src/main/resources/Template/Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanojs\eclipse-workspace-snj\snj-web-inspect\src\main\resources\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanojs\Documents\autobots-web-inspect\src\main\resources\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16035" windowHeight="7470" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16035" windowHeight="7470" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="InputLocators" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,15 @@
     <sheet name="LinkLocators" sheetId="6" r:id="rId5"/>
     <sheet name="LabelLocators" sheetId="7" r:id="rId6"/>
     <sheet name="TableLocators" sheetId="8" r:id="rId7"/>
+    <sheet name="ImageLocators" sheetId="9" r:id="rId8"/>
+    <sheet name="HeadingLocators" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="93">
   <si>
     <t>S.No</t>
   </si>
@@ -2057,8 +2059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2089,4 +2091,80 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>